<commit_message>
Update v.0.2. New additions: -Finished two pipeline cost modules -Incorporation of warning messages -First premlimenary results
</commit_message>
<xml_diff>
--- a/MatlabScripts/test_database.xlsx
+++ b/MatlabScripts/test_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsn.tno.nl\data\Projects\060\3\31986\Kluis\Werkdocumenten\WP 3\WPXX Offshore transportkosten (Wessel)\Matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F513E0D1-08F5-4FE2-891A-1D85C74011D2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E2AF3841-13D0-4FDD-BAE0-52FB539BE7DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7485" xr2:uid="{076CD78D-8EC1-4231-82DC-C83F9E042658}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="78">
   <si>
     <t>Module</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Length</t>
   </si>
   <si>
-    <t>km</t>
-  </si>
-  <si>
     <t>Flow</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>bar</t>
   </si>
   <si>
-    <t>Minimum Output Pressure</t>
-  </si>
-  <si>
     <t>Leakage</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>Safe Factor</t>
   </si>
   <si>
-    <t>mm</t>
-  </si>
-  <si>
     <t>Wall Thickness</t>
   </si>
   <si>
@@ -198,17 +189,83 @@
     <t>Project Duration</t>
   </si>
   <si>
+    <t>Minimum Pressure</t>
+  </si>
+  <si>
+    <t>Stainless Steel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mild Steel </t>
   </si>
   <si>
-    <t>Stainless Steel</t>
+    <t>S</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Pipeline Compression</t>
+  </si>
+  <si>
+    <t>Number of Trains</t>
+  </si>
+  <si>
+    <t>CO2CaptMin</t>
+  </si>
+  <si>
+    <t>kg/s</t>
+  </si>
+  <si>
+    <t>CO2CaptMax</t>
+  </si>
+  <si>
+    <t>VarAEnergy</t>
+  </si>
+  <si>
+    <t>kJe/kg</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>I0</t>
+  </si>
+  <si>
+    <t>W0</t>
+  </si>
+  <si>
+    <t>M€</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Scaling factor</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>OpexCapexRatio</t>
+  </si>
+  <si>
+    <t>Compressor Load</t>
+  </si>
+  <si>
+    <t>h/a</t>
+  </si>
+  <si>
+    <t>Electricity Costs</t>
+  </si>
+  <si>
+    <t>euro/MWh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,16 +273,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -233,16 +301,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{D99A2378-5B63-45BA-A347-77B2B1B6213A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -554,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1541D00-1096-453E-AF0B-3CB94E8DBC89}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +651,7 @@
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,13 +659,16 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -589,203 +676,208 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>80</v>
+        <v>80000</v>
       </c>
       <c r="D2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>138.4144</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>600</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>5160</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <f>40/26</f>
+        <v>1.5384615384615385</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <f>34/26</f>
+        <v>1.3076923076923077</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>0.11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>953</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>1200</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>5160</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C14">
+        <v>110</v>
+      </c>
+      <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="C12">
-        <v>190</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13">
-        <v>80</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16">
         <v>483</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15">
-        <v>550</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
+      <c r="D16" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -793,41 +885,41 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
+      <c r="B18" t="s">
+        <v>49</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>26</v>
+      <c r="B19" t="s">
+        <v>21</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -835,13 +927,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -849,13 +941,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -863,13 +955,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -877,13 +969,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C23">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -891,13 +983,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -905,13 +997,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -919,35 +1011,41 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
-        <v>34</v>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C27">
         <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B28" t="s">
-        <v>35</v>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C28">
         <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -955,10 +1053,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -966,10 +1067,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C30">
         <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -977,10 +1081,13 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C31">
         <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -988,10 +1095,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -999,10 +1109,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C33">
-        <v>1.3</v>
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,10 +1123,13 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C34">
-        <v>1.3</v>
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,10 +1137,13 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C35">
-        <v>1.5</v>
+        <v>1.3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1032,10 +1151,13 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C36">
-        <v>1.2</v>
+        <v>1.3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,10 +1165,13 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1054,10 +1179,13 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C38">
-        <v>1.5</v>
+        <v>1.2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1065,10 +1193,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1076,13 +1207,13 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C40">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,13 +1221,13 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C41">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,10 +1235,13 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C42">
-        <v>7</v>
+        <v>2.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1115,10 +1249,13 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C43">
-        <v>70</v>
+        <v>29</v>
+      </c>
+      <c r="D43" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,10 +1263,13 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C44">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,10 +1277,13 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C45">
-        <v>100</v>
+        <v>70</v>
+      </c>
+      <c r="D45" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1148,10 +1291,158 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48">
+        <v>30</v>
+      </c>
+      <c r="D48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49">
+        <v>300</v>
+      </c>
+      <c r="D49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50">
+        <v>87.85</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51">
+        <v>21.9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56">
+        <v>8000</v>
+      </c>
+      <c r="D56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57">
+        <v>40</v>
+      </c>
+      <c r="D57" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>